<commit_message>
Add CRUDD project to site
</commit_message>
<xml_diff>
--- a/bereking GIF.xlsx
+++ b/bereking GIF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Portfolio - bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C20EF6-F071-4109-8027-EF98FEFACADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECA3ED1-EDA7-420A-A9EC-CDFEACD973BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8602C4D3-C079-4959-AACE-D844266C4ADC}"/>
+    <workbookView xWindow="492" yWindow="480" windowWidth="17280" windowHeight="8976" xr2:uid="{8602C4D3-C079-4959-AACE-D844266C4ADC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>breedte</t>
+  </si>
+  <si>
+    <t>hoogte</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1CB79C-2325-4FFD-8989-9F18842C584D}">
-  <dimension ref="D9:E9"/>
+  <dimension ref="D8:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -388,13 +399,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D9">
-        <v>650</v>
+        <v>900</v>
       </c>
       <c r="E9">
         <f>D9/5*7</f>
-        <v>910</v>
+        <v>1260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>